<commit_message>
Image blob et 2e run pour Mtheo=60
</commit_message>
<xml_diff>
--- a/runs/résultats.xlsx
+++ b/runs/résultats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c6d2936775fb277a/Documents/GitHub/super_res_microscopy/runs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{58295E0C-42D0-44E4-9D44-1707A8DFA354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{58295E0C-42D0-44E4-9D44-1707A8DFA354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E63005D3-6DB5-4FDD-A4B6-5A208364F0EB}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{367CDDF0-5163-4D38-B027-23387B19740F}"/>
   </bookViews>
@@ -80,9 +80,6 @@
     <t>D estimé = 0.016570434916036304 ± 0.0007597813012299935 um^2/s et vrai D = 0.010981691 um^2/s</t>
   </si>
   <si>
-    <t>Taille estimé = 0.15089146941064271 ± 0.006918618464405832 um et vrai Taille = 0.1 um</t>
-  </si>
-  <si>
     <t>Mtheo, NA = 10, 0.25</t>
   </si>
   <si>
@@ -125,7 +122,10 @@
     <t>Taille estimé = 0.9600866553056503 ± 0.019307568444890948 um et vrai Taille = 1 um</t>
   </si>
   <si>
-    <t>Mtheo, NA = 20, 0.85</t>
+    <t>Mtheo, NA = 60, 0.85</t>
+  </si>
+  <si>
+    <t>Taille estimé = 15.089146941064271 ± 0.6918618464405832 um et vrai Taille = 10 um</t>
   </si>
 </sst>
 </file>
@@ -500,7 +500,7 @@
   <dimension ref="B2:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -577,82 +577,82 @@
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>